<commit_message>
add time diagram for wireshark packets
</commit_message>
<xml_diff>
--- a/analyser/outputs/ip info.xlsx
+++ b/analyser/outputs/ip info.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="43">
   <si>
     <t>type</t>
   </si>
@@ -22,28 +22,127 @@
     <t>location</t>
   </si>
   <si>
+    <t>media</t>
+  </si>
+  <si>
+    <t>protocol</t>
+  </si>
+  <si>
+    <t>remote</t>
+  </si>
+  <si>
     <t>Keys</t>
   </si>
   <si>
-    <t>10.0.0.191:59667 (related)</t>
-  </si>
-  <si>
-    <t>66.22.212.159:50021</t>
-  </si>
-  <si>
-    <t>10.0.0.33:50784 (related)</t>
+    <t>157.240.245.58_56442</t>
+  </si>
+  <si>
+    <t>157.240.245.58_57182</t>
+  </si>
+  <si>
+    <t>10.239.233.249_62232</t>
+  </si>
+  <si>
+    <t>10.239.233.249_52105</t>
+  </si>
+  <si>
+    <t>128.197.29.249_36960</t>
+  </si>
+  <si>
+    <t>128.197.29.249_28071</t>
+  </si>
+  <si>
+    <t>157.240.245.58_56180</t>
+  </si>
+  <si>
+    <t>10.239.233.249_9</t>
+  </si>
+  <si>
+    <t>157.240.245.58_53978</t>
+  </si>
+  <si>
+    <t>157.240.245.58_52465</t>
+  </si>
+  <si>
+    <t>157.240.245.58_55860</t>
+  </si>
+  <si>
+    <t>128.197.29.249_50060</t>
+  </si>
+  <si>
+    <t>128.197.29.249_38743</t>
+  </si>
+  <si>
+    <t>128.197.29.225_28023</t>
+  </si>
+  <si>
+    <t>10.239.25.33_55902</t>
+  </si>
+  <si>
+    <t>128.197.29.225_15914</t>
+  </si>
+  <si>
+    <t>157.240.245.58_56078</t>
+  </si>
+  <si>
+    <t>157.240.245.58_58341</t>
+  </si>
+  <si>
+    <t>128.197.29.249_25754</t>
+  </si>
+  <si>
+    <t>157.240.245.58_53239</t>
+  </si>
+  <si>
+    <t>10.239.25.33_9</t>
+  </si>
+  <si>
+    <t>128.197.29.225_36307</t>
+  </si>
+  <si>
+    <t>128.197.29.225_46635</t>
+  </si>
+  <si>
+    <t>relay</t>
+  </si>
+  <si>
+    <t>host</t>
+  </si>
+  <si>
+    <t>srflx</t>
   </si>
   <si>
     <t>prflx</t>
   </si>
   <si>
-    <t>host</t>
-  </si>
-  <si>
     <t>caller</t>
   </si>
   <si>
     <t>receiver</t>
+  </si>
+  <si>
+    <t>1_video</t>
+  </si>
+  <si>
+    <t>0_audio</t>
+  </si>
+  <si>
+    <t>udp</t>
+  </si>
+  <si>
+    <t>tcp</t>
+  </si>
+  <si>
+    <t>128.197.29.249_42250</t>
+  </si>
+  <si>
+    <t>128.197.29.249_11161</t>
+  </si>
+  <si>
+    <t>128.197.29.225_38137</t>
+  </si>
+  <si>
+    <t>128.197.29.225_3405</t>
   </si>
 </sst>
 </file>
@@ -401,15 +500,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -417,38 +516,381 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>